<commit_message>
change made to excel formule. xlookup is now lookup
</commit_message>
<xml_diff>
--- a/Logboek sifi.xlsx
+++ b/Logboek sifi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmh\Documents\GitHub\Soft_Lure_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D30263-E5F8-47D0-AB98-1BB372001CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFFDDD0-E143-42ED-B5F6-34294E4022BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D2DE36FA-96A0-4F34-A05D-A90662D87F91}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{D2DE36FA-96A0-4F34-A05D-A90662D87F91}"/>
   </bookViews>
   <sheets>
     <sheet name="logbook" sheetId="1" r:id="rId1"/>
@@ -24,28 +24,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -197,9 +175,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$USD]\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00_ ;[Red]\-0.00\ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -230,21 +223,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$USD]\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00_ ;[Red]\-0.00\ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -262,12 +240,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4225077-0106-4B98-8BF7-35C701040E3B}" name="Table1" displayName="Table1" ref="A1:M101" totalsRowShown="0">
   <autoFilter ref="A1:M101" xr:uid="{E4225077-0106-4B98-8BF7-35C701040E3B}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{E96F82EF-A2EB-489D-9AB6-5D54E28D9935}" name="Datum" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{E96F82EF-A2EB-489D-9AB6-5D54E28D9935}" name="Datum" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{2D037FAC-930D-4C44-9FD9-E0A5BE7A73D7}" name="trade"/>
     <tableColumn id="3" xr3:uid="{0517F3BF-2AC3-46CE-8030-33992A7B8D13}" name="PF Usdt"/>
-    <tableColumn id="4" xr3:uid="{7A5A41FA-A870-436A-8780-9ADB91C4E792}" name="%winst, trade" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{ECFD0288-9AFF-482E-A878-E639CF53627A}" name="Entry grote usdt" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{D4941F93-5C7B-4BD0-B778-54EA4B44E0A5}" name="% van pf" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{7A5A41FA-A870-436A-8780-9ADB91C4E792}" name="%winst, trade" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{ECFD0288-9AFF-482E-A878-E639CF53627A}" name="Entry grote usdt" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D4941F93-5C7B-4BD0-B778-54EA4B44E0A5}" name="% van pf" dataDxfId="1">
       <calculatedColumnFormula>E2 / C2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{28417176-C716-44E3-B574-52DD19FEA27D}" name="Markt trend"/>
@@ -275,7 +253,7 @@
     <tableColumn id="9" xr3:uid="{02617520-80CB-4DC0-A0C4-D59FCB6D5E0A}" name="TP1"/>
     <tableColumn id="13" xr3:uid="{D3813429-2ECA-4C30-B929-20C198DBFE3F}" name="TP2"/>
     <tableColumn id="10" xr3:uid="{DE3B3CAD-49FC-4A6A-91B2-7231BE1D2ECD}" name="BB%"/>
-    <tableColumn id="11" xr3:uid="{0A514982-9669-448B-B4B9-8B99EDD6C16D}" name="% winst op PF" dataDxfId="3">
+    <tableColumn id="11" xr3:uid="{0A514982-9669-448B-B4B9-8B99EDD6C16D}" name="% winst op PF" dataDxfId="0">
       <calculatedColumnFormula>(C3 / (C2/100)) - 100</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{6ADD19CD-73F0-43D5-9AA5-6F9DBAEBB2BC}" name="interval "/>
@@ -603,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDA3525-4390-4090-AFA4-155EB9F912D1}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -664,9 +642,9 @@
       <c r="O1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="2" t="e" cm="1">
-        <f t="array" aca="1" ref="P1" ca="1">((_xlfn.XLOOKUP(TRUE, C2:C101&lt;&gt;"",C2:C101,,,-1))/(C2/100))-100</f>
-        <v>#NAME?</v>
+      <c r="P1" s="2">
+        <f>LOOKUP(2,1/(C2:C101&lt;&gt;""),C2:C101) / (C2/100)-100</f>
+        <v>1.5713440905634997</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -2345,17 +2323,17 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L101">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2370,8 +2348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E07F031A-3A8C-43C6-A9CF-5E17A4447EA5}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2385,9 +2363,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="e" cm="1">
-        <f t="array" aca="1" ref="A2" ca="1">_xlfn.XLOOKUP(TRUE, logbook!C2:C101&lt;&gt;"",logbook!C2:C101,,,-1)</f>
-        <v>#NAME?</v>
+      <c r="A2">
+        <f>LOOKUP(2,1/(Table1[PF Usdt]&lt;&gt;""),Table1[PF Usdt])</f>
+        <v>120.23</v>
       </c>
       <c r="B2" s="8">
         <v>1.4999999999999999E-2</v>
@@ -2397,9 +2375,9 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="e">
-        <f ca="1">A2 / (100 * B2 * 1.5)</f>
-        <v>#NAME?</v>
+      <c r="C4" s="2">
+        <f>A2 / (100 * B2 * 1.5)</f>
+        <v>53.43555555555556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>